<commit_message>
barra menu y sus funcionalidades
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Excel-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1F92E477-9387-4C55-861F-49229BE02C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9B830E6C-9F0E-4FBC-B1CF-11FE2B161715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>order_id</t>
   </si>
@@ -55,12 +55,6 @@
     <t>delivery_status</t>
   </si>
   <si>
-    <t>0.0925</t>
-  </si>
-  <si>
-    <t>50.02</t>
-  </si>
-  <si>
     <t>Anna Addison</t>
   </si>
   <si>
@@ -70,12 +64,6 @@
     <t xml:space="preserve">ZW60001 </t>
   </si>
   <si>
-    <t>0.06</t>
-  </si>
-  <si>
-    <t>62.45</t>
-  </si>
-  <si>
     <t>Carol Campbell</t>
   </si>
   <si>
@@ -85,12 +73,6 @@
     <t xml:space="preserve">AB61001 </t>
   </si>
   <si>
-    <t>0.087</t>
-  </si>
-  <si>
-    <t>40.33</t>
-  </si>
-  <si>
     <t xml:space="preserve">Julia Jones </t>
   </si>
   <si>
@@ -100,12 +82,6 @@
     <t xml:space="preserve">CD62001 </t>
   </si>
   <si>
-    <t>0.0625</t>
-  </si>
-  <si>
-    <t>70.98</t>
-  </si>
-  <si>
     <t xml:space="preserve">Irene Everly </t>
   </si>
   <si>
@@ -115,9 +91,6 @@
     <t xml:space="preserve">KB63001 </t>
   </si>
   <si>
-    <t>30.45</t>
-  </si>
-  <si>
     <t>Rachel Rose</t>
   </si>
   <si>
@@ -127,9 +100,6 @@
     <t xml:space="preserve">IK64001 </t>
   </si>
   <si>
-    <t>100.2</t>
-  </si>
-  <si>
     <t>Sophie Sutton</t>
   </si>
   <si>
@@ -137,12 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">OP65001 </t>
-  </si>
-  <si>
-    <t>0.1025</t>
-  </si>
-  <si>
-    <t>58.52</t>
   </si>
   <si>
     <t>Wendy West</t>
@@ -158,7 +122,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,8 +260,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +454,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -635,9 +623,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -993,308 +986,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>50.02</v>
+      </c>
+      <c r="F2" s="4">
+        <v>49.927500000000002</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43390</v>
+      </c>
+      <c r="H2" s="2">
+        <v>43393</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1">
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="E3" s="4">
+        <v>62.45</v>
+      </c>
+      <c r="F3" s="4">
+        <v>62.39</v>
+      </c>
+      <c r="G3" s="2">
+        <v>43388</v>
+      </c>
+      <c r="H3" s="2">
+        <v>43391</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>40.33</v>
+      </c>
+      <c r="F4" s="4">
+        <v>40.242999999999995</v>
+      </c>
+      <c r="G4" s="2">
+        <v>43387</v>
+      </c>
+      <c r="H4" s="2">
         <v>43390</v>
       </c>
-      <c r="G2" s="1">
-        <v>43393</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2">
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1001</v>
-      </c>
-      <c r="B3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>70.98</v>
+      </c>
+      <c r="F5" s="4">
+        <v>70.917500000000004</v>
+      </c>
+      <c r="G5" s="2">
+        <v>43385</v>
+      </c>
+      <c r="H5" s="2">
+        <v>43388</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30.45</v>
+      </c>
+      <c r="F6" s="4">
+        <v>30.387499999999999</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43389</v>
+      </c>
+      <c r="H6" s="2">
+        <v>43392</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C7" s="4">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1">
-        <v>43388</v>
-      </c>
-      <c r="G3" s="1">
-        <v>43391</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3">
+      <c r="D7" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>100.2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>100.1375</v>
+      </c>
+      <c r="G7" s="2">
+        <v>43386</v>
+      </c>
+      <c r="H7" s="2">
+        <v>43389</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1002</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1">
-        <v>43387</v>
-      </c>
-      <c r="G4" s="1">
-        <v>43390</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1003</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="1">
-        <v>43385</v>
-      </c>
-      <c r="G5" s="1">
-        <v>43388</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="E8" s="4">
+        <v>58.52</v>
+      </c>
+      <c r="F8" s="4">
+        <v>58.417500000000004</v>
+      </c>
+      <c r="G8" s="2">
+        <v>43394</v>
+      </c>
+      <c r="H8" s="2">
+        <v>43397</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1004</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="K8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="1">
-        <v>43389</v>
-      </c>
-      <c r="G6" s="1">
-        <v>43392</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1005</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="1">
-        <v>43386</v>
-      </c>
-      <c r="G7" s="1">
-        <v>43389</v>
-      </c>
-      <c r="H7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1006</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1">
-        <v>43394</v>
-      </c>
-      <c r="G8" s="1">
-        <v>43397</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8">
+      <c r="L8" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
filtros y herramientas de revision
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -8,15 +8,62 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Excel-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9B830E6C-9F0E-4FBC-B1CF-11FE2B161715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{852BB3AF-2718-4E7D-9754-32756A88D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">order!$A$1:$L$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Santiago Quiroz Upegui</author>
+    <author>tc={663BF47F-E337-45C4-A921-FA8158EFD234}</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Santiago Quiroz Upegui:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+falta el pinchi titulo
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="1" shapeId="0">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    puto el que lo lea</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -125,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +321,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -687,6 +747,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="santiago quiroz" id="{9D2404F1-1016-431C-B5DD-BD27DA6B06D6}" userId="santiago quiroz" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -984,12 +1050,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G1" dT="2021-10-31T22:37:17.92" personId="{9D2404F1-1016-431C-B5DD-BD27DA6B06D6}" id="{663BF47F-E337-45C4-A921-FA8158EFD234}">
+    <text>puto el que lo lea</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1311,7 +1385,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
funcionalidades de un libre y hojas
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Excel-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{852BB3AF-2718-4E7D-9754-32756A88D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DC1F0DBD-EB0A-4A52-8352-9219AF4FDD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
-    <sheet name="order" sheetId="1" r:id="rId1"/>
+    <sheet name="Base de datos" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">order!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Base de datos'!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1060,10 +1061,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G9" sqref="G9:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1390,4 +1394,16 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Herramientas para trabajar con bases de datos
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Excel-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DC1F0DBD-EB0A-4A52-8352-9219AF4FDD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B4C99AC3-F1E7-42A7-84C0-45E11EBA8E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Base de datos'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Base de datos'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -26,36 +26,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Santiago Quiroz Upegui</author>
     <author>tc={663BF47F-E337-45C4-A921-FA8158EFD234}</author>
   </authors>
   <commentList>
     <comment ref="F1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Santiago Quiroz Upegui:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-falta el pinchi titulo
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="1" shapeId="0">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -68,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>order_id</t>
   </si>
@@ -173,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,13 +298,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1053,7 +1020,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G1" dT="2021-10-31T22:37:17.92" personId="{9D2404F1-1016-431C-B5DD-BD27DA6B06D6}" id="{663BF47F-E337-45C4-A921-FA8158EFD234}">
+  <threadedComment ref="F1" dT="2021-10-31T22:37:17.92" personId="{9D2404F1-1016-431C-B5DD-BD27DA6B06D6}" id="{663BF47F-E337-45C4-A921-FA8158EFD234}">
     <text>puto el que lo lea</text>
   </threadedComment>
 </ThreadedComments>
@@ -1064,10 +1031,11 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1077,17 +1045,16 @@
     <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1103,26 +1070,26 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -1138,29 +1105,26 @@
       <c r="E2" s="4">
         <v>50.02</v>
       </c>
-      <c r="F2" s="4">
-        <v>49.927500000000002</v>
+      <c r="F2" s="2">
+        <v>43390</v>
       </c>
       <c r="G2" s="2">
-        <v>43390</v>
-      </c>
-      <c r="H2" s="2">
         <v>43393</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1">
+      <c r="K2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
@@ -1176,29 +1140,26 @@
       <c r="E3" s="4">
         <v>62.45</v>
       </c>
-      <c r="F3" s="4">
-        <v>62.39</v>
+      <c r="F3" s="2">
+        <v>43388</v>
       </c>
       <c r="G3" s="2">
-        <v>43388</v>
-      </c>
-      <c r="H3" s="2">
         <v>43391</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="1">
+      <c r="K3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
@@ -1214,29 +1175,26 @@
       <c r="E4" s="4">
         <v>40.33</v>
       </c>
-      <c r="F4" s="4">
-        <v>40.242999999999995</v>
+      <c r="F4" s="2">
+        <v>43387</v>
       </c>
       <c r="G4" s="2">
-        <v>43387</v>
-      </c>
-      <c r="H4" s="2">
         <v>43390</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="1">
+      <c r="K4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
@@ -1252,29 +1210,26 @@
       <c r="E5" s="4">
         <v>70.98</v>
       </c>
-      <c r="F5" s="4">
-        <v>70.917500000000004</v>
+      <c r="F5" s="2">
+        <v>43385</v>
       </c>
       <c r="G5" s="2">
-        <v>43385</v>
-      </c>
-      <c r="H5" s="2">
         <v>43388</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="1">
+      <c r="K5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1004</v>
       </c>
@@ -1290,29 +1245,26 @@
       <c r="E6" s="4">
         <v>30.45</v>
       </c>
-      <c r="F6" s="4">
-        <v>30.387499999999999</v>
+      <c r="F6" s="2">
+        <v>43389</v>
       </c>
       <c r="G6" s="2">
-        <v>43389</v>
-      </c>
-      <c r="H6" s="2">
         <v>43392</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="1">
+      <c r="K6" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1005</v>
       </c>
@@ -1328,29 +1280,26 @@
       <c r="E7" s="4">
         <v>100.2</v>
       </c>
-      <c r="F7" s="4">
-        <v>100.1375</v>
+      <c r="F7" s="2">
+        <v>43386</v>
       </c>
       <c r="G7" s="2">
-        <v>43386</v>
-      </c>
-      <c r="H7" s="2">
         <v>43389</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="I7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="1">
+      <c r="K7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1006</v>
       </c>
@@ -1366,30 +1315,762 @@
       <c r="E8" s="4">
         <v>58.52</v>
       </c>
-      <c r="F8" s="4">
-        <v>58.417500000000004</v>
+      <c r="F8" s="2">
+        <v>43394</v>
       </c>
       <c r="G8" s="2">
+        <v>43397</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>50.02</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43390</v>
+      </c>
+      <c r="G9" s="2">
+        <v>43393</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="E10" s="4">
+        <v>62.45</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43388</v>
+      </c>
+      <c r="G10" s="2">
+        <v>43391</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>40.33</v>
+      </c>
+      <c r="F11" s="2">
+        <v>43387</v>
+      </c>
+      <c r="G11" s="2">
+        <v>43390</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>70.98</v>
+      </c>
+      <c r="F12" s="2">
+        <v>43385</v>
+      </c>
+      <c r="G12" s="2">
+        <v>43388</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <v>30.45</v>
+      </c>
+      <c r="F13" s="2">
+        <v>43389</v>
+      </c>
+      <c r="G13" s="2">
+        <v>43392</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>100.2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>43386</v>
+      </c>
+      <c r="G14" s="2">
+        <v>43389</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="E15" s="4">
+        <v>58.52</v>
+      </c>
+      <c r="F15" s="2">
         <v>43394</v>
       </c>
-      <c r="H8" s="2">
+      <c r="G15" s="2">
         <v>43397</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="1">
+      <c r="K15" s="1">
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>50.02</v>
+      </c>
+      <c r="F16" s="2">
+        <v>43390</v>
+      </c>
+      <c r="G16" s="2">
+        <v>43393</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="E17" s="4">
+        <v>62.45</v>
+      </c>
+      <c r="F17" s="2">
+        <v>43388</v>
+      </c>
+      <c r="G17" s="2">
+        <v>43391</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7</v>
+      </c>
+      <c r="C18" s="4">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E18" s="4">
+        <v>40.33</v>
+      </c>
+      <c r="F18" s="2">
+        <v>43387</v>
+      </c>
+      <c r="G18" s="2">
+        <v>43390</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B19" s="1">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E19" s="4">
+        <v>70.98</v>
+      </c>
+      <c r="F19" s="2">
+        <v>43385</v>
+      </c>
+      <c r="G19" s="2">
+        <v>43388</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B20" s="1">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>30.45</v>
+      </c>
+      <c r="F20" s="2">
+        <v>43389</v>
+      </c>
+      <c r="G20" s="2">
+        <v>43392</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>100.2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>43386</v>
+      </c>
+      <c r="G21" s="2">
+        <v>43389</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="E22" s="4">
+        <v>58.52</v>
+      </c>
+      <c r="F22" s="2">
+        <v>43394</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43397</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>50.02</v>
+      </c>
+      <c r="F23" s="2">
+        <v>43390</v>
+      </c>
+      <c r="G23" s="2">
+        <v>43393</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="E24" s="4">
+        <v>62.45</v>
+      </c>
+      <c r="F24" s="2">
+        <v>43388</v>
+      </c>
+      <c r="G24" s="2">
+        <v>43391</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B25" s="1">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>40.33</v>
+      </c>
+      <c r="F25" s="2">
+        <v>43387</v>
+      </c>
+      <c r="G25" s="2">
+        <v>43390</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B26" s="1">
+        <v>9</v>
+      </c>
+      <c r="C26" s="4">
+        <v>20</v>
+      </c>
+      <c r="D26" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E26" s="4">
+        <v>70.98</v>
+      </c>
+      <c r="F26" s="2">
+        <v>43385</v>
+      </c>
+      <c r="G26" s="2">
+        <v>43388</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="4">
+        <v>7</v>
+      </c>
+      <c r="D27" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>30.45</v>
+      </c>
+      <c r="F27" s="2">
+        <v>43389</v>
+      </c>
+      <c r="G27" s="2">
+        <v>43392</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>8</v>
+      </c>
+      <c r="D28" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>100.2</v>
+      </c>
+      <c r="F28" s="2">
+        <v>43386</v>
+      </c>
+      <c r="G28" s="2">
+        <v>43389</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="E29" s="4">
+        <v>58.52</v>
+      </c>
+      <c r="F29" s="2">
+        <v>43394</v>
+      </c>
+      <c r="G29" s="2">
+        <v>43397</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:K1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
consultar informacion con buscarv
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Excel-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B4C99AC3-F1E7-42A7-84C0-45E11EBA8E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF40981B-E2AB-4334-B0A3-B5448C04A34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base de datos" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Base de datos'!$A$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={663BF47F-E337-45C4-A921-FA8158EFD234}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -143,11 +154,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,12 +307,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -658,7 +663,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1027,15 +1032,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2070,7 +2075,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1"/>
+  <autoFilter ref="A1:K1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -2078,7 +2083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>